<commit_message>
Updated Definition Sheets now
</commit_message>
<xml_diff>
--- a/Course Project/Column Definitions for Charles.xlsx
+++ b/Course Project/Column Definitions for Charles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anaconda Python Files\GitHub\DSCD-611-Group-2-Project-Work\Course Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178D744F-8F28-46F2-A8AB-A92199FB8DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD8F15C-32A7-468D-913F-EEDD2A621F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,97 +126,97 @@
     <t>Descriptions</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Administrative Level (1 for Region, 2 for Municipality/District)</t>
-  </si>
-  <si>
-    <t>Administrative Level Id Number</t>
-  </si>
-  <si>
-    <t>PCODE for GeoSpatial Analysis</t>
-  </si>
-  <si>
-    <t>the bit depth, which determines the range of values a pixel can store, or the pixel size, which is the ground area each pixel represents (for GeoSpatial Analysis)</t>
-  </si>
-  <si>
-    <t>rainfall long term average [mm]</t>
-  </si>
-  <si>
-    <t>rainfall 1-month rolling aggregation long term average [mm]</t>
-  </si>
-  <si>
-    <t>rainfall 3-month rolling aggregation long term average [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rainfall 1-month rolling aggregation [mm] </t>
-  </si>
-  <si>
-    <t>rainfall 3-month rolling aggregation [mm]</t>
-  </si>
-  <si>
-    <t>10 day rainfall [mm]</t>
-  </si>
-  <si>
-    <t>rainfall anomaly [%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rainfall 1-month anomaly [%] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rainfall 3-month anomaly [%] </t>
-  </si>
-  <si>
-    <t>Forecast results version</t>
-  </si>
-  <si>
-    <t>11 day rainfall [mm] lagging feature by previous month</t>
-  </si>
-  <si>
-    <t>10 day rainfall [mm] lagging feature by previous dekad</t>
-  </si>
-  <si>
-    <t>rainfall 1-month anomaly [%] by previous dekad</t>
-  </si>
-  <si>
-    <t>Rainy season flag</t>
-  </si>
-  <si>
-    <t>dekad of the month - Assign dekad_of_month: 1 for 1-10, 2 for 11-20, 3 for 21+</t>
-  </si>
-  <si>
-    <t>6-month moving average (approximately 18 dekads, but using rolling window on r3h)</t>
-  </si>
-  <si>
-    <t>12-month moving average (approximately 36 dekads)</t>
-  </si>
-  <si>
-    <t>High Rainfall Flag: 1 if rfq &gt; 100%, else 0</t>
-  </si>
-  <si>
-    <t>Drought Flag: 1 if rfq &lt; -50%, else 0</t>
-  </si>
-  <si>
-    <t>Sine Transformation of Month as Cyclic Feature</t>
-  </si>
-  <si>
-    <t>Cos Transformation of Month as Cyclic Feature</t>
-  </si>
-  <si>
-    <t>Standard Deviation of rfh over the last 3 dekads. Rolling Volatility to measure the instability of rainfall intensity over the recent past.</t>
-  </si>
-  <si>
-    <t>rfh Rate of Change - Directly measures the rate of change. A large positive value indicates rapidly increasing rainfall, useful for predicting persistence.</t>
-  </si>
-  <si>
-    <t>Month of Dekad</t>
-  </si>
-  <si>
-    <t>Name of Area</t>
-  </si>
-  <si>
-    <t>Municipality Name</t>
+    <t>Dekad start date (1st, 11th, or 21st of the month) representing the 10‑day rainfall observation period.</t>
+  </si>
+  <si>
+    <t>Administrative level code for the unit (e.g., 1 = region, 2 = district or municipality).</t>
+  </si>
+  <si>
+    <t>Numeric identifier of the administrative unit in the source dataset.</t>
+  </si>
+  <si>
+    <t>Standardized administrative unit code (P-code) for the subnational area (e.g., district/municipality).</t>
+  </si>
+  <si>
+    <t>Human-readable name of the administrative unit corresponding to the PCODE.</t>
+  </si>
+  <si>
+    <t>Name of the larger municipality or metropolitan region that contains the administrative unit.</t>
+  </si>
+  <si>
+    <t>Number of satellite grid cells used to compute rainfall metrics for the unit (indicator of spatial coverage and data quality).</t>
+  </si>
+  <si>
+    <t>10‑day (dekadal) rainfall amount in millimetres for the given period.</t>
+  </si>
+  <si>
+    <t>Long-term average 10‑day rainfall (mm) for that calendar dekad at the unit (climatological mean).</t>
+  </si>
+  <si>
+    <t>1‑month rolling rainfall total (mm), typically the sum of rainfall over the last three dekads.</t>
+  </si>
+  <si>
+    <t>Long-term average 1‑month rolling rainfall (mm) for the same calendar window.</t>
+  </si>
+  <si>
+    <t>3‑month rolling rainfall total (mm), typically the sum of rainfall over the last nine dekads.</t>
+  </si>
+  <si>
+    <t>Long-term average 3‑month rolling rainfall (mm) for the same calendar window.</t>
+  </si>
+  <si>
+    <t>10‑day rainfall anomaly in percent, representing how rfh deviates from rfh_avg.</t>
+  </si>
+  <si>
+    <t>1‑month rainfall anomaly in percent, representing how r1h deviates from r1h_avg.</t>
+  </si>
+  <si>
+    <t>3‑month rainfall anomaly in percent, representing how r3h deviates from r3h_avg.</t>
+  </si>
+  <si>
+    <t>Data product type label: “forecast”, “prelim” (preliminary), or “final” observation.</t>
+  </si>
+  <si>
+    <t>Previous dekad’s 10‑day rainfall (mm) for the same PCODE (lag of 1 dekad).</t>
+  </si>
+  <si>
+    <t>10‑day rainfall (mm) from three dekads earlier (approximately one month before) for the same PCODE.</t>
+  </si>
+  <si>
+    <t>Previous dekad’s 1‑month rainfall anomaly (%) for the same PCODE.</t>
+  </si>
+  <si>
+    <t>Calendar month number (1–12) derived from the dekad date.</t>
+  </si>
+  <si>
+    <t>Position of the dekad within the month: 1 for days 1–10, 2 for days 11–20, 3 for days 21–end.</t>
+  </si>
+  <si>
+    <t>Indicator (0 = no, 1 = yes) that the dekad falls within the defined rainy season (e.g., May–October).</t>
+  </si>
+  <si>
+    <t>Sine transformation of the month value, used to encode cyclical seasonality for machine learning models.</t>
+  </si>
+  <si>
+    <t>Cosine transformation of the month value, used to encode cyclical seasonality for machine learning models.</t>
+  </si>
+  <si>
+    <t>Indicator (0 = no, 1 = yes) that the dekad is classified as drought-like based on a low rfq threshold.</t>
+  </si>
+  <si>
+    <t>Indicator (0 = no, 1 = yes) that the dekad is classified as having unusually high rainfall based on a high rfq threshold.</t>
+  </si>
+  <si>
+    <t>6‑month moving average of the 3‑month rolling rainfall (r3h) for each PCODE, capturing medium-term trends.</t>
+  </si>
+  <si>
+    <t>12‑month moving average of the 3‑month rolling rainfall (r3h) for each PCODE, capturing long-term trends.</t>
+  </si>
+  <si>
+    <t>Rolling standard deviation of 10‑day rainfall over the last three dekads, indicating short-term rainfall variability.</t>
+  </si>
+  <si>
+    <t>Change in 10‑day rainfall from the previous dekad, computed as rfh − rfh_lag_1 (mm).</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -836,7 +836,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +852,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>